<commit_message>
The project goes well, but there is no Error Hadling yet
</commit_message>
<xml_diff>
--- a/Proyecto/Junior - UNO/Input/Information.xlsx
+++ b/Proyecto/Junior - UNO/Input/Information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivan_\OneDrive\Documentos\Power Automate\Repo\Proyecto\Junior - UNO\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0113819E-0BB7-4EA1-9016-3F237BAFEC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A117C55-E209-4AE1-8EE1-A4E649F8929B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D14A7F66-EE23-4BA6-BE76-9BB7CF8472ED}"/>
   </bookViews>
@@ -458,7 +458,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F16" sqref="A7:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>